<commit_message>
metodos para eliminar y para sumar las ventas y compras
</commit_message>
<xml_diff>
--- a/rom/Animals/Wilds.xlsx
+++ b/rom/Animals/Wilds.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -80,7 +80,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -914,6 +914,742 @@
         <v>7</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" t="s">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" t="s">
+        <v>7</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>7</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F41" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>7</v>
+      </c>
+      <c r="G44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+      <c r="E45" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>7</v>
+      </c>
+      <c r="G45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+      <c r="E46" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>7</v>
+      </c>
+      <c r="G50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>7</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" t="s">
+        <v>7</v>
+      </c>
+      <c r="G51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>7</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" t="s">
+        <v>7</v>
+      </c>
+      <c r="F53" t="s">
+        <v>7</v>
+      </c>
+      <c r="G53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+      <c r="E54" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>7</v>
+      </c>
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>7</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>7</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>7</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" t="s">
+        <v>7</v>
+      </c>
+      <c r="F60" t="s">
+        <v>7</v>
+      </c>
+      <c r="G60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>7</v>
+      </c>
+      <c r="B61" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" t="s">
+        <v>7</v>
+      </c>
+      <c r="F61" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" t="s">
+        <v>7</v>
+      </c>
+      <c r="F62" t="s">
+        <v>7</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" t="s">
+        <v>7</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" t="s">
+        <v>7</v>
+      </c>
+      <c r="F64" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" t="s">
+        <v>7</v>
+      </c>
+      <c r="F65" t="s">
+        <v>7</v>
+      </c>
+      <c r="G65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
+        <v>7</v>
+      </c>
+      <c r="F66" t="s">
+        <v>7</v>
+      </c>
+      <c r="G66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>7</v>
+      </c>
+      <c r="F67" t="s">
+        <v>7</v>
+      </c>
+      <c r="G67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>7</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" t="s">
+        <v>7</v>
+      </c>
+      <c r="G68" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>